<commit_message>
Clarifications on CAR data by Mark Grace
</commit_message>
<xml_diff>
--- a/Excel files/Ad-hoc/QuestionsSentToMark_4Oct_Krish.xlsx
+++ b/Excel files/Ad-hoc/QuestionsSentToMark_4Oct_Krish.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akl0407\Desktop\Academia\GitHub\STAT390_LegalAid_Fall2025\Excel files\Ad-hoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059826DA-7E26-4131-B88E-7D061D210F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CB8CCE-55AA-44A8-A9DF-4CE4F9BAF47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="679" firstSheet="1" activeTab="1" xr2:uid="{607C3898-A061-43F2-B8EC-A6C01FB58344}"/>
   </bookViews>
   <sheets>
     <sheet name="termination reason" sheetId="4" state="hidden" r:id="rId1"/>
-    <sheet name="customer left" sheetId="3" r:id="rId2"/>
-    <sheet name="agent left" sheetId="2" r:id="rId3"/>
-    <sheet name="sys disconnect" sheetId="5" r:id="rId4"/>
-    <sheet name="multiple terminations" sheetId="6" r:id="rId5"/>
-    <sheet name="Popular numbers" sheetId="7" r:id="rId6"/>
+    <sheet name="Questions &amp; Answers" sheetId="8" r:id="rId2"/>
+    <sheet name="customer left" sheetId="3" r:id="rId3"/>
+    <sheet name="agent left" sheetId="2" r:id="rId4"/>
+    <sheet name="sys disconnect" sheetId="5" r:id="rId5"/>
+    <sheet name="multiple terminations" sheetId="6" r:id="rId6"/>
+    <sheet name="Popular numbers" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="193">
   <si>
     <t>Contact Session ID</t>
   </si>
@@ -582,6 +583,405 @@
   </si>
   <si>
     <t>Scenario 2: What is intake outdial EP?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Question 1: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scenario 1: Customer seems to have left just after selecting the language. Can we say that they left while they were listening to the menu options?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Answer 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Scenario 1: Assuming by “menu”, you mean the language selection menu, then yes.  In the case of that LAC main number call in April, the caller heard one second of the language selection menu, so I expect the caller hung up while listening to the language selection menu itself.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Question 2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scenario 2: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Customer left as they were calling during closed hours. However, the field "System disconnected the contact" indicates the disconnection in case of a call during closed hours. Does this mean that the customer disconnected before the system was about to disconnect the call?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Answer 2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  In which field did you see “System disconnected the contact”.  That one looks like the caller hung up during the closed menu (IVR-ClosedMenu-{{CallerLanugage}}.wav.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Question 4: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scenario 4: The customer was transferred to the staff directory. They left after being in that queue for a minute. Did the customer leave without finding the contact of the staff they intended, or is there no way to tell if they found the contact or not?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Answer 4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  As with scenario 3, this transfer queue/CBT (both called “Staff Directory English Transfer”) would have resulted in a blind transfer to a Webex Calling auto-attendant at x2302.  From there, WxCC doesn’t know what the caller did, so Webex Calling reports would be required.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Question 5: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scenario 5:  I believe in this case the customer heard the voicemail that LegalAid doesn't serve Tenant Deterrence, and then disconnected.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Answer 5:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  The caller pressed option 4 on the tenant menu (from Housing), heard the tenant deterrence message/menu, and was routed back to the tenant menu, where the caller disconnected.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Question 6: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scenario 5:  I believe in this case the customer heard the voicemail that LegalAid doesn't serve Tenant Deterrence, and then disconnected.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Answer 6:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  The caller pressed option 4 on the tenant menu (from Housing), heard the tenant deterrence message/menu, and was routed back to the tenant menu, where the caller disconnected.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Question 3: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scenario 3: What is CBT agent? The customer left after being for 8 minutes on "Front Desk Transfer". Does this mean that the customer were in a queue for front desk and then dropped off? Will this be an example of an abandoned call?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Answer 3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  You will see “CBT” as the answering agent for any Capacity Based Team, which is where we transfer from Webex Contact Center to Webex Calling.  For example, when we blind transfer a call from a WxCC IVR/menu to the front desk, we “queue” the call for a “Front Desk Transfer” queue where the only assigned team is a Capacity Based Team called “Front Desk Transfer”.  Agents sign into Agent Based Teams, but Capacity Based Teams immediately transfer to the DN configured on that CBT.  For the “Front Desk Transfer” team, that configured transfer DN is x6300.  Unfortunately, that’s where WxCC reporting ends and; you’d need to marry it with detailed call history (CDRs) from Webex Calling to determine what ultimately happened with a call transferred outside of WxCC.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Question 7: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Scenario 1: The customer is listening to a voicemail of criminal records. Then why is there an agent, and they are leaving?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Answer 7: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Once the caller is transferred to Webex Calling via the “Criminal Records Voicemail Transfer” queue/CBT, we don’t know what happens with the call.  My best guess between transfers that resulted in “Customer Left” vs. transfers that ended with “Agent Left” is the terminating side (PSTN side disconnect vs. Webex side disconnect).</t>
+    </r>
+  </si>
+  <si>
+    <t>On the sheet named "customer left", there are 6 scenarios, and below are the questions asked and answers obtained on each of the scenario:</t>
+  </si>
+  <si>
+    <t>On the sheet named "agent left", there are 6 scenarios, and below are the questions asked and answers obtained on each of the scenario:</t>
+  </si>
+  <si>
+    <t>Purple text: Important for understanding data</t>
+  </si>
+  <si>
+    <t>Agent left</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Question 8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Scenario 2: Does "Intake Outdial EP" indicate that this is a callback to a customer? But those are indicated as "Courtsey Callback EP". What is the difference between the two? It seems like Flora Fell talked to the customer for 10 minutes and then left. Is that correct? Also, after the agent leaves they come back again, which is not clear why.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Answer 8:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This was a manually dialed (ad-hoc) outbound call from Flora to a PSTN number (708-452-xxxx).  For whatever reason, WxCC calls them “outdials”, but they’re different from courtesy callbacks, where the callback is waiting in a queue.  In this case, Flora manually dialed the number from the agent desktop, it rang for 18 seconds, and successfully connected to that PSTN number where it lasted for a little over 10 minutes.  Flora ended the call and then entered the wrapup state for four seconds.  That “DisconnectContact” activity you see prior to the “SetCallerID” activity is an unused activity in the main portion of the outdial flow used on all ad-hoc outbound calls.  It doesn’t do anything, but is required.  We’re using the “SetCallerID” activity in the event portion of the outdial flow to ensure the appropriate outbound caller ID.  After that, the outdial/outbound call flow is completed and call progress is now determined by the two parties (transfer, hold, conference, call termination, etc.).</t>
+    </r>
+  </si>
+  <si>
+    <t>Questions sent by Krish; Answers provided by Mark Grace</t>
   </si>
 </sst>
 </file>
@@ -592,7 +992,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -619,6 +1019,28 @@
       <sz val="12"/>
       <name val="Source Sans Pro"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -663,7 +1085,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -675,6 +1097,25 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1242,11 +1683,264 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A5B109F-1D4B-4447-A751-044ED95B3761}">
+  <dimension ref="A2:Q17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="12.68359375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="62.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:17" ht="76.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="1:17" ht="121.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" spans="1:17" ht="81.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" ht="67.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" ht="63.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:17" ht="15.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+    </row>
+    <row r="12" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="67.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+    </row>
+    <row r="17" spans="1:16" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A16:P16"/>
+    <mergeCell ref="A17:P17"/>
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="A6:P6"/>
+    <mergeCell ref="A7:P7"/>
+    <mergeCell ref="A8:P8"/>
+    <mergeCell ref="A9:P9"/>
+    <mergeCell ref="A10:P10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331DC657-FD3A-4378-9471-2138B2FA97E5}">
   <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2880,12 +3574,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F316077-71B5-4BE2-A7C5-047BA3CED120}">
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3488,7 +4182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E77537F-D178-490F-9F96-ADCD9F684540}">
   <dimension ref="A1:J20"/>
   <sheetViews>
@@ -3824,7 +4518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6240E722-7DB7-4705-9BAA-9B033C26DB80}">
   <dimension ref="A1:J55"/>
   <sheetViews>
@@ -4961,12 +5655,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E99A146-3D06-475A-9292-A8960AB107A0}">
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5021,6 +5715,9 @@
       <c r="B4">
         <v>53614</v>
       </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">

</xml_diff>